<commit_message>
Tue Aug 29 21:30:42 CST 2023
</commit_message>
<xml_diff>
--- a/笔记/知识点梳理/攻击.xlsx
+++ b/笔记/知识点梳理/攻击.xlsx
@@ -19,7 +19,7 @@
     <author>chloroplast</author>
   </authors>
   <commentList>
-    <comment ref="B50" authorId="0">
+    <comment ref="B51" authorId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="292">
   <si>
     <t>分类</t>
   </si>
@@ -320,6 +320,114 @@
   </si>
   <si>
     <t>反编译</t>
+  </si>
+  <si>
+    <t>Oracle Padding攻击</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">通常被称为“Padding Oracle攻击”，是针对加密系统中块加密算法的一种攻击。它利用了一个“Oracle”（预言机），这个Oracle会告诉攻击者他提供的一个加密块是否具有有效的填充。虽然这看起来信息量很小，但利用这个反馈，攻击者可以逐字节地解密数据。
+1. </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>背景：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">在块加密中，数据经常需要被填充到一个固定大小的块。例如，AES加密使用的块大小是128位。如果要加密的数据不是128位的倍数，那么就需要填充数据。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2. 预言机：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">攻击者利用了一个Oracle，通常是一个服务或功能，该服务会根据是否正确解密数据块（具有有效填充）来提供不同的响应。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>3. 攻击过程：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+ 3.1 攻击者发送一系列的篡改过的加密消息给Oracle。
+ 3.2 根据Oracle的反应，攻击者可以判断出消息的某部分是否具有有效的填充。
+ 3.3 通过逐字节地改变加密的数据并观察Oracle的反应，攻击者最终可以解密整个消息，而不需要知道加密密钥。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>4. 结果：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>攻击者通过这种方法可以逐步解密整个消息，这大大减少了破解所需的尝试次数。</t>
+    </r>
+  </si>
+  <si>
+    <t>根据是否正确解密数据块（具有有效填充）来提供不同的响应进行破解</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. 不区分填充错误和其他解密错误的响应。
+2. 使用认证加密（AE）或认证加密与关联数据（AEAD）模式，如GCM或ChaCha20-Poly1305，以确保在解密之前首先验证数据的完整性。
+3. 避免使用已知存在漏洞的加密模式，如CBC模式，或确保在使用时采取适当的安全措施。
+</t>
   </si>
   <si>
     <t>社会工程</t>
@@ -1005,12 +1113,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1034,6 +1142,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1042,8 +1157,78 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1058,14 +1243,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1086,22 +1279,7 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1110,71 +1288,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1228,7 +1344,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1240,13 +1446,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1258,43 +1470,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1306,37 +1482,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1354,55 +1500,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1468,6 +1584,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -1500,35 +1640,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1550,168 +1681,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="18" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1743,6 +1859,9 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1752,16 +1871,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2089,12 +2205,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G114"/>
+  <dimension ref="A1:G115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A105" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C110" sqref="C110"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.671875" defaultRowHeight="40" customHeight="1" outlineLevelCol="6"/>
@@ -2103,7 +2219,7 @@
     <col min="2" max="2" width="17.0625" style="1" customWidth="1"/>
     <col min="3" max="3" width="112.3671875" style="1" customWidth="1"/>
     <col min="4" max="4" width="24.734375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="51.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="70.703125" style="1" customWidth="1"/>
     <col min="6" max="6" width="23.3046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="56.8984375" style="1" customWidth="1"/>
     <col min="8" max="8" width="90.234375" style="1" customWidth="1"/>
@@ -2619,353 +2735,357 @@
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" s="1" customFormat="1" customHeight="1" spans="1:7">
+    <row r="37" s="1" customFormat="1" ht="185" customHeight="1" spans="1:7">
       <c r="A37" s="8"/>
       <c r="B37" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
+      <c r="C37" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>94</v>
+      </c>
       <c r="F37" s="4"/>
       <c r="G37" s="4"/>
     </row>
     <row r="38" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A38" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="A38" s="8"/>
       <c r="B38" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="D38" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="4"/>
+    </row>
+    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:7">
+      <c r="A39" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="39" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A39" s="9"/>
-      <c r="B39" s="4"/>
       <c r="C39" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="D39" s="4"/>
+      <c r="D39" s="4" t="s">
+        <v>99</v>
+      </c>
       <c r="E39" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="G39" s="4" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="40" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A40" s="9"/>
-      <c r="B40" s="4" t="s">
-        <v>100</v>
-      </c>
+      <c r="A40" s="10"/>
+      <c r="B40" s="4"/>
       <c r="C40" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
+      <c r="E40" s="4" t="s">
+        <v>103</v>
+      </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
     </row>
-    <row r="41" s="1" customFormat="1" ht="62" customHeight="1" spans="1:7">
-      <c r="A41" s="9"/>
+    <row r="41" s="1" customFormat="1" customHeight="1" spans="1:7">
+      <c r="A41" s="10"/>
       <c r="B41" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="D41" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="E41" s="4" t="s">
         <v>105</v>
       </c>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="4" t="s">
+      <c r="G41" s="4"/>
+    </row>
+    <row r="42" s="1" customFormat="1" ht="62" customHeight="1" spans="1:7">
+      <c r="A42" s="10"/>
+      <c r="B42" s="4" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="42" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
-      <c r="A42" s="9"/>
-      <c r="B42" s="4" t="s">
+      <c r="C42" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="D42" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="D42" s="10" t="s">
+      <c r="E42" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="G42" s="4" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="43" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
-      <c r="A43" s="9"/>
+      <c r="A43" s="10"/>
       <c r="B43" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="10"/>
+        <v>112</v>
+      </c>
+      <c r="D43" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
     </row>
     <row r="44" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
-      <c r="A44" s="9"/>
+      <c r="A44" s="10"/>
       <c r="B44" s="4" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="D44" s="10"/>
+        <v>115</v>
+      </c>
+      <c r="D44" s="11"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="4"/>
     </row>
     <row r="45" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
-      <c r="A45" s="9"/>
+      <c r="A45" s="10"/>
       <c r="B45" s="4" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D45" s="10"/>
+        <v>117</v>
+      </c>
+      <c r="D45" s="11"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="4"/>
     </row>
     <row r="46" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
-      <c r="A46" s="9"/>
+      <c r="A46" s="10"/>
       <c r="B46" s="4" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D46" s="10"/>
+        <v>119</v>
+      </c>
+      <c r="D46" s="11"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="4"/>
     </row>
     <row r="47" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
-      <c r="A47" s="9"/>
+      <c r="A47" s="10"/>
       <c r="B47" s="4" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="D47" s="10"/>
+        <v>121</v>
+      </c>
+      <c r="D47" s="11"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="4"/>
     </row>
-    <row r="48" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A48" s="9"/>
+    <row r="48" s="1" customFormat="1" ht="47" customHeight="1" spans="1:7">
+      <c r="A48" s="10"/>
       <c r="B48" s="4" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="D48" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="E48" s="4" t="s">
         <v>123</v>
       </c>
+      <c r="D48" s="11"/>
+      <c r="E48" s="4"/>
       <c r="F48" s="4"/>
       <c r="G48" s="4"/>
     </row>
     <row r="49" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A49" s="9"/>
-      <c r="B49" s="4"/>
+      <c r="A49" s="10"/>
+      <c r="B49" s="4" t="s">
+        <v>124</v>
+      </c>
       <c r="C49" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="D49" s="11"/>
-      <c r="E49" s="4"/>
+        <v>125</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>127</v>
+      </c>
       <c r="F49" s="4"/>
       <c r="G49" s="4"/>
     </row>
-    <row r="50" s="1" customFormat="1" ht="69" customHeight="1" spans="1:7">
-      <c r="A50" s="9"/>
-      <c r="B50" s="4" t="s">
-        <v>125</v>
-      </c>
+    <row r="50" s="1" customFormat="1" customHeight="1" spans="1:7">
+      <c r="A50" s="10"/>
+      <c r="B50" s="4"/>
       <c r="C50" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="D50" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E50" s="4" t="s">
         <v>128</v>
       </c>
+      <c r="D50" s="12"/>
+      <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="4" t="s">
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" s="1" customFormat="1" ht="69" customHeight="1" spans="1:7">
+      <c r="A51" s="10"/>
+      <c r="B51" s="4" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="51" s="1" customFormat="1" ht="60" customHeight="1" spans="1:7">
-      <c r="A51" s="9"/>
-      <c r="B51" s="4" t="s">
+      <c r="C51" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="C51" s="4" t="s">
+      <c r="D51" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="D51" s="4" t="s">
+      <c r="E51" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="E51" s="4" t="s">
+      <c r="F51" s="4"/>
+      <c r="G51" s="4" t="s">
         <v>133</v>
       </c>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-    </row>
-    <row r="52" s="1" customFormat="1" ht="138" customHeight="1" spans="1:7">
-      <c r="A52" s="9"/>
+    </row>
+    <row r="52" s="1" customFormat="1" ht="60" customHeight="1" spans="1:7">
+      <c r="A52" s="10"/>
       <c r="B52" s="4" t="s">
         <v>134</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D52" s="4"/>
+      <c r="D52" s="4" t="s">
+        <v>136</v>
+      </c>
       <c r="E52" s="4" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A53" s="9"/>
+      <c r="G52" s="4"/>
+    </row>
+    <row r="53" s="1" customFormat="1" ht="138" customHeight="1" spans="1:7">
+      <c r="A53" s="10"/>
       <c r="B53" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="4" t="s">
+        <v>139</v>
+      </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
+      <c r="G53" s="4" t="s">
+        <v>141</v>
+      </c>
     </row>
     <row r="54" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A54" s="9"/>
+      <c r="A54" s="10"/>
       <c r="B54" s="4" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
+      <c r="E54" s="4" t="s">
+        <v>143</v>
+      </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
     </row>
     <row r="55" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A55" s="9"/>
+      <c r="A55" s="10"/>
       <c r="B55" s="4" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
-      <c r="E55" s="4" t="s">
-        <v>142</v>
-      </c>
+      <c r="E55" s="4"/>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
     </row>
     <row r="56" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A56" s="9"/>
+      <c r="A56" s="10"/>
       <c r="B56" s="4" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
       <c r="E56" s="4" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
     </row>
     <row r="57" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A57" s="9"/>
+      <c r="A57" s="10"/>
       <c r="B57" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>146</v>
-      </c>
+        <v>147</v>
+      </c>
+      <c r="C57" s="4"/>
       <c r="D57" s="4"/>
       <c r="E57" s="4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="F57" s="4"/>
       <c r="G57" s="4"/>
     </row>
     <row r="58" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A58" s="9"/>
+      <c r="A58" s="10"/>
       <c r="B58" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C58" s="4"/>
+        <v>149</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>150</v>
+      </c>
       <c r="D58" s="4"/>
       <c r="E58" s="4" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="F58" s="4"/>
       <c r="G58" s="4"/>
     </row>
     <row r="59" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A59" s="9"/>
+      <c r="A59" s="10"/>
       <c r="B59" s="4" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
+      <c r="E59" s="4" t="s">
+        <v>153</v>
+      </c>
       <c r="F59" s="4"/>
       <c r="G59" s="4"/>
     </row>
     <row r="60" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A60" s="9"/>
+      <c r="A60" s="10"/>
       <c r="B60" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>152</v>
-      </c>
+        <v>154</v>
+      </c>
+      <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="4"/>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
     </row>
     <row r="61" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A61" s="9"/>
+      <c r="A61" s="10"/>
       <c r="B61" s="4" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D61" s="4"/>
       <c r="E61" s="4"/>
@@ -2973,14 +3093,12 @@
       <c r="G61" s="4"/>
     </row>
     <row r="62" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A62" s="9" t="s">
-        <v>137</v>
-      </c>
+      <c r="A62" s="10"/>
       <c r="B62" s="4" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="D62" s="4"/>
       <c r="E62" s="4"/>
@@ -2988,12 +3106,14 @@
       <c r="G62" s="4"/>
     </row>
     <row r="63" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A63" s="9"/>
+      <c r="A63" s="10" t="s">
+        <v>141</v>
+      </c>
       <c r="B63" s="4" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D63" s="4"/>
       <c r="E63" s="4"/>
@@ -3001,12 +3121,12 @@
       <c r="G63" s="4"/>
     </row>
     <row r="64" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A64" s="9"/>
+      <c r="A64" s="10"/>
       <c r="B64" s="4" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="D64" s="4"/>
       <c r="E64" s="4"/>
@@ -3014,40 +3134,40 @@
       <c r="G64" s="4"/>
     </row>
     <row r="65" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A65" s="9"/>
+      <c r="A65" s="10"/>
       <c r="B65" s="4" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="D65" s="4"/>
-      <c r="E65" s="4" t="s">
-        <v>163</v>
-      </c>
+      <c r="E65" s="4"/>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
     </row>
     <row r="66" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A66" s="9"/>
+      <c r="A66" s="10"/>
       <c r="B66" s="4" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
+      <c r="E66" s="4" t="s">
+        <v>167</v>
+      </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
     </row>
     <row r="67" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A67" s="9"/>
+      <c r="A67" s="10"/>
       <c r="B67" s="4" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D67" s="4"/>
       <c r="E67" s="4"/>
@@ -3055,87 +3175,85 @@
       <c r="G67" s="4"/>
     </row>
     <row r="68" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A68" s="12" t="s">
-        <v>168</v>
-      </c>
+      <c r="A68" s="10"/>
       <c r="B68" s="4" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="D68" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E68" s="4" t="s">
-        <v>172</v>
-      </c>
+      <c r="D68" s="4"/>
+      <c r="E68" s="4"/>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
     </row>
     <row r="69" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A69" s="13"/>
+      <c r="A69" s="14" t="s">
+        <v>172</v>
+      </c>
       <c r="B69" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
+      <c r="C69" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>175</v>
+      </c>
       <c r="E69" s="4" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
     </row>
     <row r="70" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A70" s="12" t="s">
-        <v>175</v>
-      </c>
+      <c r="A70" s="15"/>
       <c r="B70" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="C70" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="D70" s="4" t="s">
+      <c r="C70" s="4"/>
+      <c r="D70" s="4"/>
+      <c r="E70" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="E70" s="4"/>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
     </row>
     <row r="71" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A71" s="14"/>
+      <c r="A71" s="14" t="s">
+        <v>179</v>
+      </c>
       <c r="B71" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
+        <v>180</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>182</v>
+      </c>
       <c r="E71" s="4"/>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
     </row>
     <row r="72" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A72" s="13"/>
+      <c r="A72" s="16"/>
       <c r="B72" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>180</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C72" s="4"/>
       <c r="D72" s="4"/>
       <c r="E72" s="4"/>
       <c r="F72" s="4"/>
       <c r="G72" s="4"/>
     </row>
     <row r="73" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A73" s="9" t="s">
-        <v>181</v>
-      </c>
+      <c r="A73" s="15"/>
       <c r="B73" s="4" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="D73" s="4"/>
       <c r="E73" s="4"/>
@@ -3143,14 +3261,14 @@
       <c r="G73" s="4"/>
     </row>
     <row r="74" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A74" s="9" t="s">
-        <v>116</v>
+      <c r="A74" s="10" t="s">
+        <v>185</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="D74" s="4"/>
       <c r="E74" s="4"/>
@@ -3158,12 +3276,14 @@
       <c r="G74" s="4"/>
     </row>
     <row r="75" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A75" s="9"/>
+      <c r="A75" s="10" t="s">
+        <v>120</v>
+      </c>
       <c r="B75" s="4" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="D75" s="4"/>
       <c r="E75" s="4"/>
@@ -3171,40 +3291,40 @@
       <c r="G75" s="4"/>
     </row>
     <row r="76" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A76" s="9"/>
+      <c r="A76" s="10"/>
       <c r="B76" s="4" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="D76" s="4" t="s">
-        <v>190</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="D76" s="4"/>
       <c r="E76" s="4"/>
       <c r="F76" s="4"/>
       <c r="G76" s="4"/>
     </row>
     <row r="77" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A77" s="9"/>
+      <c r="A77" s="10"/>
       <c r="B77" s="4" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="D77" s="4"/>
+        <v>193</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="E77" s="4"/>
       <c r="F77" s="4"/>
       <c r="G77" s="4"/>
     </row>
     <row r="78" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A78" s="9"/>
+      <c r="A78" s="10"/>
       <c r="B78" s="4" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="4"/>
@@ -3212,12 +3332,12 @@
       <c r="G78" s="4"/>
     </row>
     <row r="79" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A79" s="9"/>
+      <c r="A79" s="10"/>
       <c r="B79" s="4" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="4"/>
@@ -3225,55 +3345,55 @@
       <c r="G79" s="4"/>
     </row>
     <row r="80" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A80" s="9"/>
+      <c r="A80" s="10"/>
       <c r="B80" s="4" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="D80" s="4" t="s">
-        <v>199</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="D80" s="4"/>
       <c r="E80" s="4"/>
       <c r="F80" s="4"/>
       <c r="G80" s="4"/>
     </row>
     <row r="81" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A81" s="9"/>
+      <c r="A81" s="10"/>
       <c r="B81" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C81" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="D81" s="4"/>
+      <c r="C81" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>203</v>
+      </c>
       <c r="E81" s="4"/>
       <c r="F81" s="4"/>
-      <c r="G81" s="4" t="s">
-        <v>202</v>
-      </c>
+      <c r="G81" s="4"/>
     </row>
     <row r="82" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A82" s="9"/>
+      <c r="A82" s="10"/>
       <c r="B82" s="4" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="C82" s="5" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="D82" s="4"/>
       <c r="E82" s="4"/>
       <c r="F82" s="4"/>
-      <c r="G82" s="4"/>
+      <c r="G82" s="4" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="83" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A83" s="9"/>
+      <c r="A83" s="10"/>
       <c r="B83" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="C83" s="4" t="s">
-        <v>206</v>
+        <v>207</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>208</v>
       </c>
       <c r="D83" s="4"/>
       <c r="E83" s="4"/>
@@ -3281,12 +3401,12 @@
       <c r="G83" s="4"/>
     </row>
     <row r="84" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A84" s="9"/>
+      <c r="A84" s="10"/>
       <c r="B84" s="4" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="D84" s="4"/>
       <c r="E84" s="4"/>
@@ -3294,40 +3414,40 @@
       <c r="G84" s="4"/>
     </row>
     <row r="85" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A85" s="9"/>
+      <c r="A85" s="10"/>
       <c r="B85" s="4" t="s">
-        <v>209</v>
+        <v>211</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="D85" s="4"/>
       <c r="E85" s="4"/>
       <c r="F85" s="4"/>
-      <c r="G85" s="4" t="s">
-        <v>211</v>
-      </c>
+      <c r="G85" s="4"/>
     </row>
     <row r="86" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A86" s="9"/>
+      <c r="A86" s="10"/>
       <c r="B86" s="4" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="D86" s="4"/>
       <c r="E86" s="4"/>
       <c r="F86" s="4"/>
-      <c r="G86" s="4"/>
+      <c r="G86" s="4" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="87" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A87" s="9"/>
+      <c r="A87" s="10"/>
       <c r="B87" s="4" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D87" s="4"/>
       <c r="E87" s="4"/>
@@ -3335,12 +3455,12 @@
       <c r="G87" s="4"/>
     </row>
     <row r="88" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A88" s="9"/>
+      <c r="A88" s="10"/>
       <c r="B88" s="4" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="D88" s="4"/>
       <c r="E88" s="4"/>
@@ -3348,12 +3468,12 @@
       <c r="G88" s="4"/>
     </row>
     <row r="89" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A89" s="9"/>
+      <c r="A89" s="10"/>
       <c r="B89" s="4" t="s">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
@@ -3361,12 +3481,12 @@
       <c r="G89" s="4"/>
     </row>
     <row r="90" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A90" s="9"/>
+      <c r="A90" s="10"/>
       <c r="B90" s="4" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>221</v>
+        <v>223</v>
       </c>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
@@ -3374,14 +3494,12 @@
       <c r="G90" s="4"/>
     </row>
     <row r="91" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A91" s="15" t="s">
-        <v>222</v>
-      </c>
+      <c r="A91" s="10"/>
       <c r="B91" s="4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
@@ -3389,123 +3507,121 @@
       <c r="G91" s="4"/>
     </row>
     <row r="92" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A92" s="16"/>
+      <c r="A92" s="14" t="s">
+        <v>226</v>
+      </c>
       <c r="B92" s="4" t="s">
-        <v>33</v>
+        <v>227</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
       <c r="F92" s="4"/>
-      <c r="G92" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="93" s="1" customFormat="1" ht="55" customHeight="1" spans="1:7">
+      <c r="G92" s="4"/>
+    </row>
+    <row r="93" s="1" customFormat="1" customHeight="1" spans="1:7">
       <c r="A93" s="16"/>
       <c r="B93" s="4" t="s">
-        <v>227</v>
+        <v>33</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>228</v>
-      </c>
-      <c r="D93" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="E93" s="4" t="s">
-        <v>230</v>
-      </c>
+      <c r="D93" s="4"/>
+      <c r="E93" s="4"/>
       <c r="F93" s="4"/>
       <c r="G93" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="94" s="1" customFormat="1" ht="55" customHeight="1" spans="1:7">
       <c r="A94" s="16"/>
-      <c r="B94" s="4"/>
+      <c r="B94" s="4" t="s">
+        <v>231</v>
+      </c>
       <c r="C94" s="4" t="s">
         <v>232</v>
       </c>
       <c r="D94" s="4" t="s">
         <v>233</v>
       </c>
-      <c r="E94" s="4"/>
+      <c r="E94" s="4" t="s">
+        <v>234</v>
+      </c>
       <c r="F94" s="4"/>
       <c r="G94" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="95" s="1" customFormat="1" ht="55" customHeight="1" spans="1:7">
       <c r="A95" s="16"/>
       <c r="B95" s="4"/>
       <c r="C95" s="4" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>236</v>
-      </c>
-      <c r="E95" s="4" t="s">
         <v>237</v>
       </c>
+      <c r="E95" s="4"/>
       <c r="F95" s="4"/>
-      <c r="G95" s="4"/>
+      <c r="G95" s="4" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="96" s="1" customFormat="1" ht="55" customHeight="1" spans="1:7">
       <c r="A96" s="16"/>
       <c r="B96" s="4"/>
       <c r="C96" s="4" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D96" s="4" t="s">
-        <v>239</v>
-      </c>
-      <c r="E96" s="4"/>
+        <v>240</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>241</v>
+      </c>
       <c r="F96" s="4"/>
       <c r="G96" s="4"/>
     </row>
-    <row r="97" s="1" customFormat="1" ht="105" customHeight="1" spans="1:7">
+    <row r="97" s="1" customFormat="1" ht="55" customHeight="1" spans="1:7">
       <c r="A97" s="16"/>
-      <c r="B97" s="4" t="s">
-        <v>240</v>
-      </c>
+      <c r="B97" s="4"/>
       <c r="C97" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="D97" s="4" t="s">
-        <v>242</v>
-      </c>
-      <c r="E97" s="4" t="s">
         <v>243</v>
       </c>
+      <c r="E97" s="4"/>
       <c r="F97" s="4"/>
-      <c r="G97" s="4" t="s">
+      <c r="G97" s="4"/>
+    </row>
+    <row r="98" s="1" customFormat="1" ht="105" customHeight="1" spans="1:7">
+      <c r="A98" s="16"/>
+      <c r="B98" s="4" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="98" s="1" customFormat="1" ht="83" customHeight="1" spans="1:7">
-      <c r="A98" s="16"/>
-      <c r="B98" s="10" t="s">
+      <c r="C98" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="D98" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="D98" s="4" t="s">
+      <c r="E98" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="E98" s="4" t="s">
+      <c r="F98" s="4"/>
+      <c r="G98" s="4" t="s">
         <v>248</v>
       </c>
-      <c r="F98" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="G98" s="4"/>
     </row>
     <row r="99" s="1" customFormat="1" ht="83" customHeight="1" spans="1:7">
       <c r="A99" s="16"/>
-      <c r="B99" s="11"/>
+      <c r="B99" s="11" t="s">
+        <v>249</v>
+      </c>
       <c r="C99" s="4" t="s">
         <v>250</v>
       </c>
@@ -3515,89 +3631,91 @@
       <c r="E99" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="F99" s="4"/>
-      <c r="G99" s="4" t="s">
+      <c r="F99" s="4" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="100" s="1" customFormat="1" ht="54" customHeight="1" spans="1:7">
+      <c r="G99" s="4"/>
+    </row>
+    <row r="100" s="1" customFormat="1" ht="83" customHeight="1" spans="1:7">
       <c r="A100" s="16"/>
-      <c r="B100" s="11" t="s">
+      <c r="B100" s="12"/>
+      <c r="C100" s="4" t="s">
         <v>254</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="D100" s="4" t="s">
         <v>255</v>
       </c>
-      <c r="D100" s="4"/>
-      <c r="E100" s="4"/>
+      <c r="E100" s="4" t="s">
+        <v>256</v>
+      </c>
       <c r="F100" s="4"/>
       <c r="G100" s="4" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="101" s="1" customFormat="1" customHeight="1" spans="1:7">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="101" s="1" customFormat="1" ht="54" customHeight="1" spans="1:7">
       <c r="A101" s="16"/>
-      <c r="B101" s="4" t="s">
-        <v>257</v>
+      <c r="B101" s="12" t="s">
+        <v>258</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
       <c r="F101" s="4"/>
-      <c r="G101" s="4"/>
-    </row>
-    <row r="102" s="1" customFormat="1" ht="57" customHeight="1" spans="1:7">
+      <c r="G101" s="4" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="102" s="1" customFormat="1" customHeight="1" spans="1:7">
       <c r="A102" s="16"/>
       <c r="B102" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="C102" s="4"/>
+        <v>261</v>
+      </c>
+      <c r="C102" s="4" t="s">
+        <v>262</v>
+      </c>
       <c r="D102" s="4"/>
-      <c r="E102" s="4" t="s">
-        <v>260</v>
-      </c>
+      <c r="E102" s="4"/>
       <c r="F102" s="4"/>
       <c r="G102" s="4"/>
     </row>
-    <row r="103" s="1" customFormat="1" customHeight="1" spans="1:7">
+    <row r="103" s="1" customFormat="1" ht="57" customHeight="1" spans="1:7">
       <c r="A103" s="16"/>
       <c r="B103" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>262</v>
-      </c>
+        <v>263</v>
+      </c>
+      <c r="C103" s="4"/>
       <c r="D103" s="4"/>
-      <c r="E103" s="4"/>
+      <c r="E103" s="4" t="s">
+        <v>264</v>
+      </c>
       <c r="F103" s="4"/>
       <c r="G103" s="4"/>
     </row>
     <row r="104" s="1" customFormat="1" customHeight="1" spans="1:7">
       <c r="A104" s="16"/>
       <c r="B104" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="C104" s="4"/>
+        <v>265</v>
+      </c>
+      <c r="C104" s="4" t="s">
+        <v>266</v>
+      </c>
       <c r="D104" s="4"/>
-      <c r="E104" s="4" t="s">
-        <v>264</v>
-      </c>
+      <c r="E104" s="4"/>
       <c r="F104" s="4"/>
       <c r="G104" s="4"/>
     </row>
-    <row r="105" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
+    <row r="105" s="1" customFormat="1" customHeight="1" spans="1:7">
       <c r="A105" s="16"/>
       <c r="B105" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="C105" s="4" t="s">
-        <v>266</v>
-      </c>
+        <v>267</v>
+      </c>
+      <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="F105" s="4"/>
       <c r="G105" s="4"/>
@@ -3605,14 +3723,14 @@
     <row r="106" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
       <c r="A106" s="16"/>
       <c r="B106" s="4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="D106" s="4"/>
       <c r="E106" s="4" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
@@ -3620,23 +3738,25 @@
     <row r="107" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
       <c r="A107" s="16"/>
       <c r="B107" s="4" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="D107" s="4"/>
-      <c r="E107" s="4"/>
+      <c r="E107" s="4" t="s">
+        <v>274</v>
+      </c>
       <c r="F107" s="4"/>
       <c r="G107" s="4"/>
     </row>
     <row r="108" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
       <c r="A108" s="16"/>
       <c r="B108" s="4" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
@@ -3646,10 +3766,10 @@
     <row r="109" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
       <c r="A109" s="16"/>
       <c r="B109" s="4" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
@@ -3659,40 +3779,38 @@
     <row r="110" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
       <c r="A110" s="16"/>
       <c r="B110" s="4" t="s">
-        <v>277</v>
+        <v>279</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>278</v>
+        <v>280</v>
       </c>
       <c r="D110" s="4"/>
-      <c r="E110" s="4" t="s">
-        <v>279</v>
-      </c>
+      <c r="E110" s="4"/>
       <c r="F110" s="4"/>
       <c r="G110" s="4"/>
     </row>
     <row r="111" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
       <c r="A111" s="16"/>
       <c r="B111" s="4" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="D111" s="4"/>
-      <c r="E111" s="4"/>
+      <c r="E111" s="4" t="s">
+        <v>283</v>
+      </c>
       <c r="F111" s="4"/>
       <c r="G111" s="4"/>
     </row>
-    <row r="112" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A112" s="9" t="s">
-        <v>282</v>
-      </c>
+    <row r="112" s="1" customFormat="1" ht="51" customHeight="1" spans="1:7">
+      <c r="A112" s="16"/>
       <c r="B112" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
@@ -3700,12 +3818,14 @@
       <c r="G112" s="4"/>
     </row>
     <row r="113" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A113" s="9"/>
+      <c r="A113" s="10" t="s">
+        <v>286</v>
+      </c>
       <c r="B113" s="4" t="s">
-        <v>285</v>
-      </c>
-      <c r="C113" s="17" t="s">
-        <v>286</v>
+        <v>287</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>288</v>
       </c>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
@@ -3713,39 +3833,52 @@
       <c r="G113" s="4"/>
     </row>
     <row r="114" s="1" customFormat="1" customHeight="1" spans="1:7">
-      <c r="A114" s="9"/>
+      <c r="A114" s="10"/>
       <c r="B114" s="4" t="s">
-        <v>287</v>
-      </c>
-      <c r="C114" s="4"/>
+        <v>289</v>
+      </c>
+      <c r="C114" s="17" t="s">
+        <v>290</v>
+      </c>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
       <c r="F114" s="4"/>
       <c r="G114" s="4"/>
     </row>
+    <row r="115" s="1" customFormat="1" customHeight="1" spans="1:7">
+      <c r="A115" s="10"/>
+      <c r="B115" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="C115" s="4"/>
+      <c r="D115" s="4"/>
+      <c r="E115" s="4"/>
+      <c r="F115" s="4"/>
+      <c r="G115" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="21">
     <mergeCell ref="A2:A14"/>
-    <mergeCell ref="A15:A37"/>
-    <mergeCell ref="A38:A61"/>
-    <mergeCell ref="A62:A67"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="A70:A72"/>
-    <mergeCell ref="A74:A90"/>
-    <mergeCell ref="A91:A111"/>
-    <mergeCell ref="A112:A114"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B48:B49"/>
-    <mergeCell ref="B93:B96"/>
-    <mergeCell ref="B98:B99"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="D48:D49"/>
-    <mergeCell ref="E93:E94"/>
-    <mergeCell ref="E95:E96"/>
-    <mergeCell ref="G38:G39"/>
-    <mergeCell ref="G41:G49"/>
-    <mergeCell ref="G50:G51"/>
-    <mergeCell ref="G94:G96"/>
+    <mergeCell ref="A15:A38"/>
+    <mergeCell ref="A39:A62"/>
+    <mergeCell ref="A63:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A75:A91"/>
+    <mergeCell ref="A92:A112"/>
+    <mergeCell ref="A113:A115"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B94:B97"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="D49:D50"/>
+    <mergeCell ref="E94:E95"/>
+    <mergeCell ref="E96:E97"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="G42:G50"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="G95:G97"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -3756,7 +3889,7 @@
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <commentList sheetStid="1">
-    <comment s:ref="B50" rgbClr="000000"/>
+    <comment s:ref="B51" rgbClr="000000"/>
   </commentList>
 </comments>
 </file>

</xml_diff>